<commit_message>
language based data entry excel
</commit_message>
<xml_diff>
--- a/examples/schema_json_examples/chicken_example_data_entry.xlsx
+++ b/examples/schema_json_examples/chicken_example_data_entry.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -93,16 +93,16 @@
     <t>Required</t>
   </si>
   <si>
-    <t>Character Encoding</t>
-  </si>
-  <si>
-    <t>OL: Format</t>
+    <t>Entry</t>
   </si>
   <si>
     <t>Entry Code</t>
   </si>
   <si>
-    <t>Entry</t>
+    <t>Character Encoding</t>
+  </si>
+  <si>
+    <t>OL: Format</t>
   </si>
   <si>
     <t>Age</t>
@@ -117,13 +117,7 @@
     <t>Bird Age</t>
   </si>
   <si>
-    <t>Age de l'animal</t>
-  </si>
-  <si>
     <t>age of bird in days</t>
-  </si>
-  <si>
-    <t>Age de l'animal compté en jours</t>
   </si>
   <si>
     <t>utf-8</t>
@@ -138,13 +132,7 @@
     <t>Breast Weight</t>
   </si>
   <si>
-    <t>Poids de la poitrine</t>
-  </si>
-  <si>
     <t>Breast weight in grams</t>
-  </si>
-  <si>
-    <t>Poids de la poitrine en gramme</t>
   </si>
   <si>
     <t>Gram</t>
@@ -162,22 +150,16 @@
     <t>Type of breed</t>
   </si>
   <si>
-    <t>type de race</t>
-  </si>
-  <si>
     <t>information on the type of breed</t>
   </si>
   <si>
-    <t>informations sur le type de race</t>
-  </si>
-  <si>
-    <t>[A-Z]{15}</t>
+    <t>B:Brahma|S:Silkie</t>
   </si>
   <si>
     <t>B|S</t>
   </si>
   <si>
-    <t>B:Brahma|S:Silkie</t>
+    <t>[A-Z]{15}</t>
   </si>
   <si>
     <t>Farm</t>
@@ -186,13 +168,7 @@
     <t>Farm Letter Indentifier</t>
   </si>
   <si>
-    <t>Lettre itenditifant la ferme</t>
-  </si>
-  <si>
     <t>a letter given to the farm for identification</t>
-  </si>
-  <si>
-    <t>Letter assignee a chaque ferme pour identification</t>
   </si>
   <si>
     <t>Glucose</t>
@@ -201,13 +177,7 @@
     <t>Glucose Concentration</t>
   </si>
   <si>
-    <t>Concentration de glucose</t>
-  </si>
-  <si>
     <t>glucose content in mmol/L</t>
-  </si>
-  <si>
-    <t>Concentration de glucose en mmol/L</t>
   </si>
   <si>
     <t>Y</t>
@@ -219,13 +189,7 @@
     <t>Lipase Content</t>
   </si>
   <si>
-    <t>Concentration de lipase</t>
-  </si>
-  <si>
     <t>lipase content in U/L</t>
-  </si>
-  <si>
-    <t>Concentration de glucose en U/L</t>
   </si>
   <si>
     <t>LiveWt</t>
@@ -234,13 +198,7 @@
     <t>Live Weight</t>
   </si>
   <si>
-    <t>Poids vif</t>
-  </si>
-  <si>
     <t>weight in grams at 28 days</t>
-  </si>
-  <si>
-    <t>Poids vif à 28 jours en gramme</t>
   </si>
   <si>
     <t>Lookup tables</t>
@@ -692,16 +650,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O41"/>
+  <dimension ref="A2:M41"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="5" width="17" customWidth="1"/>
-    <col min="6" max="8" width="20" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="11" width="15" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -804,7 +762,7 @@
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -818,34 +776,28 @@
         <v>22</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
@@ -861,26 +813,20 @@
       <c r="E27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>31</v>
@@ -889,103 +835,85 @@
         <v>32</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="4" t="s">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="B30" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>31</v>
@@ -994,33 +922,27 @@
         <v>32</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1029,33 +951,27 @@
         <v>32</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>31</v>
@@ -1064,55 +980,49 @@
         <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1139,25 +1049,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25"/>
@@ -2186,22 +2096,22 @@
         <v>30</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>